<commit_message>
Handle null-like values in xlsx files
</commit_message>
<xml_diff>
--- a/test/compatibility/test_data/logical-conditions.xlsx
+++ b/test/compatibility/test_data/logical-conditions.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuba/HotNoBackup/hyperformula/test/compatibility/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuba/HotNoBackup/hyperformula/test/compatibility/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6311CCAA-1A17-7E4C-838F-164A314FBA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D854713-887C-CC46-85C9-D3A0E2301477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{29B9C796-F800-B64F-9596-CCA94A0D2F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -154,7 +154,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F33"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,10 +755,10 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
-        <v>45306</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -770,10 +770,10 @@
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1">
-        <v>45342</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -785,8 +785,8 @@
       <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
-        <v>45301</v>
+      <c r="C18">
+        <v>3</v>
       </c>
       <c r="D18" t="b">
         <f>NOT(TRUE)</f>
@@ -801,8 +801,8 @@
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1">
-        <v>45352</v>
+      <c r="C19">
+        <v>4</v>
       </c>
       <c r="D19" t="b">
         <f>NOT(FALSE)</f>
@@ -817,8 +817,8 @@
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1">
-        <v>45306</v>
+      <c r="C20">
+        <v>5</v>
       </c>
       <c r="D20" t="b">
         <f>AND(TRUE,TRUE,FALSE)</f>

</xml_diff>

<commit_message>
Add test:compatibility to npm run test script
</commit_message>
<xml_diff>
--- a/test/compatibility/test_data/logical-conditions.xlsx
+++ b/test/compatibility/test_data/logical-conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuba/HotNoBackup/hyperformula/test/compatibility/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D854713-887C-CC46-85C9-D3A0E2301477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761B6801-142B-F442-93F5-CD3F0FC4D6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{29B9C796-F800-B64F-9596-CCA94A0D2F6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Test Values</t>
   </si>
@@ -83,13 +83,7 @@
     <t>Apple</t>
   </si>
   <si>
-    <t>=TRUE AND FALSE</t>
-  </si>
-  <si>
     <t>Banana</t>
-  </si>
-  <si>
-    <t>=TRUE OR FALSE</t>
   </si>
   <si>
     <t>Cherry</t>
@@ -758,8 +752,9 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
+      <c r="D16" s="1" t="b">
+        <f>AND(TRUE, FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,13 +763,14 @@
         <v>Match Found</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>17</v>
+      <c r="D17" s="1" t="b">
+        <f>OR(TRUE, FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -799,7 +795,7 @@
         <v>Complex Check</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -815,25 +811,25 @@
         <v>Same Signs</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="b">
-        <f>AND(TRUE,TRUE,FALSE)</f>
-        <v>0</v>
+        <f>_xlfn.XOR(TRUE, FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -908,13 +904,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
         <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -933,7 +929,7 @@
         <v>Is Blank</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C31" t="str">
         <f>IF(B5&lt;&gt;0,"Non-Zero","Zero")</f>

</xml_diff>